<commit_message>
Add multi-post and subreddit scraping, add requirements for binder link
</commit_message>
<xml_diff>
--- a/data/single_post_reddit_comments.xlsx
+++ b/data/single_post_reddit_comments.xlsx
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>45265.3721412037</v>
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>45267.94893518519</v>
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>45265.37</v>
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-10</v>
+        <v>-8</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>45265.59289351852</v>
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>45265.61190972223</v>
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>45265.91684027778</v>
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>45265.53335648148</v>

</xml_diff>